<commit_message>
Cleaned up values in the appendix
</commit_message>
<xml_diff>
--- a/GDP_Appendix5.xlsx
+++ b/GDP_Appendix5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bltho\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bltho\source\repos\GDP_Appendix5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DFF572-EF73-4C74-A565-02CD298D148A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0332395-C7A4-45E4-8270-1EAA6655EF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="236">
   <si>
     <t>Track Name</t>
   </si>
@@ -758,9 +758,6 @@
   </si>
   <si>
     <t>C</t>
-  </si>
-  <si>
-    <t>Average Time to 1km</t>
   </si>
   <si>
     <t>Track Section</t>
@@ -1178,11 +1175,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF87"/>
+  <dimension ref="A1:Y85"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC57" sqref="AC57"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1209,7 @@
     <col min="25" max="25" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1288,11 +1285,8 @@
       <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1341,7 +1335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1415,12 +1409,8 @@
       <c r="Y3" t="s">
         <v>35</v>
       </c>
-      <c r="AB3">
-        <f t="shared" ref="AB3:AB63" si="0">J3/D3</f>
-        <v>4.8054765712931706</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1497,12 +1487,8 @@
       <c r="Y4" t="s">
         <v>36</v>
       </c>
-      <c r="AB4">
-        <f t="shared" si="0"/>
-        <v>4.2472262952101651</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1556,7 +1542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1633,12 +1619,8 @@
       <c r="Y6" t="s">
         <v>40</v>
       </c>
-      <c r="AB6">
-        <f t="shared" si="0"/>
-        <v>4.4784966578383152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1704,12 +1686,8 @@
       <c r="Y7" t="s">
         <v>41</v>
       </c>
-      <c r="AB7">
-        <f t="shared" si="0"/>
-        <v>5.0799678805913748</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1783,12 +1761,8 @@
       <c r="Y8" t="s">
         <v>44</v>
       </c>
-      <c r="AB8">
-        <f t="shared" si="0"/>
-        <v>3.3851384393265498</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1865,12 +1839,8 @@
       <c r="Y9" t="s">
         <v>46</v>
       </c>
-      <c r="AB9">
-        <f t="shared" si="0"/>
-        <v>4.8623632777478925</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1947,12 +1917,8 @@
       <c r="Y10" t="s">
         <v>47</v>
       </c>
-      <c r="AB10">
-        <f t="shared" si="0"/>
-        <v>4.2144691134269747</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -2006,7 +1972,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -2060,7 +2026,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -2114,7 +2080,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2188,12 +2154,8 @@
       <c r="Y14" t="s">
         <v>59</v>
       </c>
-      <c r="AB14">
-        <f t="shared" si="0"/>
-        <v>4.4526082892604029</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -2267,12 +2229,8 @@
       <c r="Y15" t="s">
         <v>61</v>
       </c>
-      <c r="AB15">
-        <f t="shared" si="0"/>
-        <v>4.6693569107534199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -2349,12 +2307,8 @@
       <c r="Y16" t="s">
         <v>64</v>
       </c>
-      <c r="AB16">
-        <f t="shared" si="0"/>
-        <v>4.7226114370785535</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -2428,17 +2382,13 @@
       <c r="Y17" t="s">
         <v>66</v>
       </c>
-      <c r="AB17">
-        <f t="shared" si="0"/>
-        <v>4.3038714116890304</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -2512,12 +2462,8 @@
       <c r="Y20" t="s">
         <v>34</v>
       </c>
-      <c r="AB20">
-        <f t="shared" si="0"/>
-        <v>3.7797462350290525</v>
-      </c>
-    </row>
-    <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2594,12 +2540,8 @@
       <c r="Y21" t="s">
         <v>69</v>
       </c>
-      <c r="AB21">
-        <f t="shared" si="0"/>
-        <v>3.2061368179241625</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -2650,7 +2592,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2704,7 +2646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2781,12 +2723,8 @@
       <c r="Y24" t="s">
         <v>76</v>
       </c>
-      <c r="AB24">
-        <f t="shared" si="0"/>
-        <v>4.5152507995943516</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2840,7 +2778,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>80</v>
       </c>
@@ -2914,12 +2852,8 @@
       <c r="Y26" t="s">
         <v>81</v>
       </c>
-      <c r="AB26">
-        <f t="shared" si="0"/>
-        <v>4.1830039719511598</v>
-      </c>
-    </row>
-    <row r="27" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>82</v>
       </c>
@@ -2996,17 +2930,13 @@
       <c r="Y27" t="s">
         <v>83</v>
       </c>
-      <c r="AB27">
-        <f t="shared" si="0"/>
-        <v>4.3727620470337927</v>
-      </c>
-    </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -3023,7 +2953,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="7">
-        <f t="shared" ref="F30:F35" si="1">SUM(G30:I30)</f>
+        <f t="shared" ref="F30:F35" si="0">SUM(G30:I30)</f>
         <v>263.459</v>
       </c>
       <c r="G30" s="7">
@@ -3036,11 +2966,11 @@
         <v>71.319000000000003</v>
       </c>
       <c r="J30" s="7">
-        <f t="shared" ref="J30:J36" si="2">AVERAGE(G30:I30)</f>
+        <f t="shared" ref="J30:J36" si="1">AVERAGE(G30:I30)</f>
         <v>87.819666666666663</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" ref="K30:K36" si="3">LARGE(L30:N30, 1)</f>
+        <f t="shared" ref="K30:K36" si="2">LARGE(L30:N30, 1)</f>
         <v>1574</v>
       </c>
       <c r="L30" s="9">
@@ -3053,7 +2983,7 @@
         <v>1574</v>
       </c>
       <c r="O30" s="9">
-        <f t="shared" ref="O30:O36" si="4">AVERAGE(L30:N30)</f>
+        <f t="shared" ref="O30:O36" si="3">AVERAGE(L30:N30)</f>
         <v>1322.3333333333333</v>
       </c>
       <c r="P30" s="10">
@@ -3080,12 +3010,8 @@
       <c r="Y30" t="s">
         <v>87</v>
       </c>
-      <c r="AB30">
-        <f t="shared" si="0"/>
-        <v>3.8190766108574326</v>
-      </c>
-    </row>
-    <row r="31" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -3102,7 +3028,7 @@
         <v>24</v>
       </c>
       <c r="F31" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>108.01400000000001</v>
       </c>
       <c r="G31" s="7">
@@ -3115,11 +3041,11 @@
         <v>33.6</v>
       </c>
       <c r="J31" s="7">
+        <f t="shared" si="1"/>
+        <v>36.004666666666672</v>
+      </c>
+      <c r="K31" s="9">
         <f t="shared" si="2"/>
-        <v>36.004666666666672</v>
-      </c>
-      <c r="K31" s="9">
-        <f t="shared" si="3"/>
         <v>972</v>
       </c>
       <c r="L31" s="9">
@@ -3132,7 +3058,7 @@
         <v>972</v>
       </c>
       <c r="O31" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>890.66666666666663</v>
       </c>
       <c r="P31" s="10">
@@ -3162,12 +3088,8 @@
       <c r="Y31" t="s">
         <v>89</v>
       </c>
-      <c r="AB31">
-        <f t="shared" si="0"/>
-        <v>4.451615562149688</v>
-      </c>
-    </row>
-    <row r="32" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>90</v>
       </c>
@@ -3184,7 +3106,7 @@
         <v>24</v>
       </c>
       <c r="F32" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>185.32500000000002</v>
       </c>
       <c r="G32" s="7">
@@ -3197,11 +3119,11 @@
         <v>58.779000000000003</v>
       </c>
       <c r="J32" s="7">
+        <f t="shared" si="1"/>
+        <v>61.775000000000006</v>
+      </c>
+      <c r="K32" s="9">
         <f t="shared" si="2"/>
-        <v>61.775000000000006</v>
-      </c>
-      <c r="K32" s="9">
-        <f t="shared" si="3"/>
         <v>1211</v>
       </c>
       <c r="L32" s="9">
@@ -3214,7 +3136,7 @@
         <v>1211</v>
       </c>
       <c r="O32" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1037</v>
       </c>
       <c r="P32" s="10">
@@ -3244,12 +3166,8 @@
       <c r="Y32" t="s">
         <v>91</v>
       </c>
-      <c r="AB32">
-        <f t="shared" si="0"/>
-        <v>4.2819019893255703</v>
-      </c>
-    </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>93</v>
       </c>
@@ -3266,7 +3184,7 @@
         <v>24</v>
       </c>
       <c r="F33" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>197.25799999999998</v>
       </c>
       <c r="G33" s="7">
@@ -3279,11 +3197,11 @@
         <v>72.540000000000006</v>
       </c>
       <c r="J33" s="7">
+        <f t="shared" si="1"/>
+        <v>65.752666666666656</v>
+      </c>
+      <c r="K33" s="9">
         <f t="shared" si="2"/>
-        <v>65.752666666666656</v>
-      </c>
-      <c r="K33" s="9">
-        <f t="shared" si="3"/>
         <v>1947</v>
       </c>
       <c r="L33" s="9">
@@ -3296,7 +3214,7 @@
         <v>1914</v>
       </c>
       <c r="O33" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1894.6666666666667</v>
       </c>
       <c r="P33" s="10">
@@ -3323,12 +3241,8 @@
       <c r="Y33" t="s">
         <v>94</v>
       </c>
-      <c r="AB33">
-        <f t="shared" si="0"/>
-        <v>3.1278026194780071</v>
-      </c>
-    </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>95</v>
       </c>
@@ -3345,7 +3259,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>116.25900000000001</v>
       </c>
       <c r="G34" s="7">
@@ -3358,11 +3272,11 @@
         <v>37.020000000000003</v>
       </c>
       <c r="J34" s="7">
+        <f t="shared" si="1"/>
+        <v>38.753000000000007</v>
+      </c>
+      <c r="K34" s="9">
         <f t="shared" si="2"/>
-        <v>38.753000000000007</v>
-      </c>
-      <c r="K34" s="9">
-        <f t="shared" si="3"/>
         <v>1013</v>
       </c>
       <c r="L34" s="9">
@@ -3375,7 +3289,7 @@
         <v>1013</v>
       </c>
       <c r="O34" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>954.66666666666663</v>
       </c>
       <c r="P34" s="10">
@@ -3402,12 +3316,8 @@
       <c r="Y34" t="s">
         <v>96</v>
       </c>
-      <c r="AB34">
-        <f t="shared" si="0"/>
-        <v>4.328976764968723</v>
-      </c>
-    </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -3424,7 +3334,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>201.92099999999999</v>
       </c>
       <c r="G35" s="7">
@@ -3437,11 +3347,11 @@
         <v>43.801000000000002</v>
       </c>
       <c r="J35" s="7">
+        <f t="shared" si="1"/>
+        <v>67.307000000000002</v>
+      </c>
+      <c r="K35" s="9">
         <f t="shared" si="2"/>
-        <v>67.307000000000002</v>
-      </c>
-      <c r="K35" s="9">
-        <f t="shared" si="3"/>
         <v>2264</v>
       </c>
       <c r="L35" s="9">
@@ -3454,7 +3364,7 @@
         <v>2264</v>
       </c>
       <c r="O35" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1754</v>
       </c>
       <c r="P35" s="10">
@@ -3481,12 +3391,8 @@
       <c r="Y35" t="s">
         <v>98</v>
       </c>
-      <c r="AB35">
-        <f t="shared" si="0"/>
-        <v>3.3923189355375234</v>
-      </c>
-    </row>
-    <row r="36" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>99</v>
       </c>
@@ -3509,11 +3415,11 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="7">
+        <f t="shared" si="1"/>
+        <v>36.747</v>
+      </c>
+      <c r="K36" s="9">
         <f t="shared" si="2"/>
-        <v>36.747</v>
-      </c>
-      <c r="K36" s="9">
-        <f t="shared" si="3"/>
         <v>800</v>
       </c>
       <c r="L36" s="9">
@@ -3522,7 +3428,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
       <c r="O36" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>800</v>
       </c>
       <c r="P36" s="13">
@@ -3552,12 +3458,8 @@
       <c r="Y36" t="s">
         <v>100</v>
       </c>
-      <c r="AB36">
-        <f t="shared" si="0"/>
-        <v>4.6937028994763059</v>
-      </c>
-    </row>
-    <row r="37" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>102</v>
       </c>
@@ -3611,7 +3513,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -3685,12 +3587,8 @@
       <c r="Y38" t="s">
         <v>106</v>
       </c>
-      <c r="AB38">
-        <f t="shared" si="0"/>
-        <v>4.2805110155129711</v>
-      </c>
-    </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>107</v>
       </c>
@@ -3764,12 +3662,8 @@
       <c r="Y39" t="s">
         <v>108</v>
       </c>
-      <c r="AB39">
-        <f t="shared" si="0"/>
-        <v>4.4640640640640639</v>
-      </c>
-    </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -3843,12 +3737,8 @@
       <c r="Y40" t="s">
         <v>111</v>
       </c>
-      <c r="AB40">
-        <f t="shared" si="0"/>
-        <v>4.0755085243974127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>112</v>
       </c>
@@ -3922,12 +3812,8 @@
       <c r="Y41" t="s">
         <v>113</v>
       </c>
-      <c r="AB41">
-        <f t="shared" si="0"/>
-        <v>3.8326736798250169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -4001,17 +3887,13 @@
       <c r="Y42" t="s">
         <v>114</v>
       </c>
-      <c r="AB42">
-        <f t="shared" si="0"/>
-        <v>4.3868502581755591</v>
-      </c>
-    </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>116</v>
       </c>
@@ -4065,7 +3947,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>119</v>
       </c>
@@ -4142,12 +4024,8 @@
       <c r="Y46" t="s">
         <v>121</v>
       </c>
-      <c r="AB46">
-        <f t="shared" si="0"/>
-        <v>4.4517278785061221</v>
-      </c>
-    </row>
-    <row r="47" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>122</v>
       </c>
@@ -4201,7 +4079,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>125</v>
       </c>
@@ -4255,7 +4133,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>128</v>
       </c>
@@ -4309,7 +4187,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>131</v>
       </c>
@@ -4383,12 +4261,8 @@
       <c r="Y50" t="s">
         <v>132</v>
       </c>
-      <c r="AB50">
-        <f t="shared" si="0"/>
-        <v>4.2211871583647707</v>
-      </c>
-    </row>
-    <row r="51" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>133</v>
       </c>
@@ -4442,7 +4316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>135</v>
       </c>
@@ -4519,12 +4393,8 @@
       <c r="Y52" t="s">
         <v>137</v>
       </c>
-      <c r="AB52">
-        <f t="shared" si="0"/>
-        <v>4.3833684090779821</v>
-      </c>
-    </row>
-    <row r="53" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>138</v>
       </c>
@@ -4578,7 +4448,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>141</v>
       </c>
@@ -4629,12 +4499,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>144</v>
       </c>
@@ -4684,23 +4554,8 @@
       <c r="Y57" t="s">
         <v>145</v>
       </c>
-      <c r="AC57" t="s">
-        <v>225</v>
-      </c>
-      <c r="AD57" cm="1">
-        <f t="array" ref="AD57">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC57,"")))</f>
-        <v>815</v>
-      </c>
-      <c r="AE57" cm="1">
-        <f t="array" ref="AE57">AD57/SUM(LEN($Y$2:$Y$1000))</f>
-        <v>0.3479931682322801</v>
-      </c>
-      <c r="AF57">
-        <f>AE57*100</f>
-        <v>34.799316823228011</v>
-      </c>
-    </row>
-    <row r="58" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>146</v>
       </c>
@@ -4753,23 +4608,8 @@
       <c r="Y58" t="s">
         <v>148</v>
       </c>
-      <c r="AC58" t="s">
-        <v>226</v>
-      </c>
-      <c r="AD58" cm="1">
-        <f t="array" ref="AD58">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC58,"")))</f>
-        <v>388</v>
-      </c>
-      <c r="AE58" cm="1">
-        <f t="array" ref="AE58">AD58/SUM(LEN($Y$3:$Y$1001))</f>
-        <v>0.16862233811386354</v>
-      </c>
-      <c r="AF58">
-        <f t="shared" ref="AF58:AF63" si="5">AE58*100</f>
-        <v>16.862233811386353</v>
-      </c>
-    </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>149</v>
       </c>
@@ -4819,23 +4659,8 @@
       <c r="Y59" t="s">
         <v>150</v>
       </c>
-      <c r="AC59" t="s">
-        <v>227</v>
-      </c>
-      <c r="AD59" cm="1">
-        <f t="array" ref="AD59">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC59,"")))</f>
-        <v>176</v>
-      </c>
-      <c r="AE59" cm="1">
-        <f t="array" ref="AE59">AD59/SUM(LEN($Y$4:$Y$1002))</f>
-        <v>7.8048780487804878E-2</v>
-      </c>
-      <c r="AF59">
-        <f t="shared" si="5"/>
-        <v>7.8048780487804876</v>
-      </c>
-    </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>151</v>
       </c>
@@ -4885,23 +4710,8 @@
       <c r="Y60" t="s">
         <v>152</v>
       </c>
-      <c r="AC60" t="s">
-        <v>228</v>
-      </c>
-      <c r="AD60" cm="1">
-        <f t="array" ref="AD60">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC60,"")))</f>
-        <v>388</v>
-      </c>
-      <c r="AE60" cm="1">
-        <f t="array" ref="AE60">AD60/SUM(LEN(Y5:Y1003))</f>
-        <v>0.17628350749659247</v>
-      </c>
-      <c r="AF60">
-        <f t="shared" si="5"/>
-        <v>17.628350749659248</v>
-      </c>
-    </row>
-    <row r="61" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>153</v>
       </c>
@@ -4928,7 +4738,7 @@
         <v>104.935</v>
       </c>
       <c r="K61" s="9">
-        <f t="shared" ref="K61" si="6">LARGE(L61:N61, 1)</f>
+        <f t="shared" ref="K61" si="4">LARGE(L61:N61, 1)</f>
         <v>1000</v>
       </c>
       <c r="L61" s="9">
@@ -4967,27 +4777,8 @@
       <c r="Y61" t="s">
         <v>155</v>
       </c>
-      <c r="AB61">
-        <f t="shared" si="0"/>
-        <v>4.49670037709976</v>
-      </c>
-      <c r="AC61" t="s">
-        <v>229</v>
-      </c>
-      <c r="AD61" cm="1">
-        <f t="array" ref="AD61">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC61,"")))</f>
-        <v>100</v>
-      </c>
-      <c r="AE61" cm="1">
-        <f t="array" ref="AE61">AD61/SUM(LEN($Y$6:$Y$1004))</f>
-        <v>4.6533271288971612E-2</v>
-      </c>
-      <c r="AF61">
-        <f t="shared" si="5"/>
-        <v>4.6533271288971614</v>
-      </c>
-    </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>156</v>
       </c>
@@ -5021,7 +4812,7 @@
         <v>84.059666666666672</v>
       </c>
       <c r="K62" s="9">
-        <f t="shared" ref="K62:K63" si="7">LARGE(L62:N62, 1)</f>
+        <f t="shared" ref="K62:K63" si="5">LARGE(L62:N62, 1)</f>
         <v>1978</v>
       </c>
       <c r="L62" s="9">
@@ -5061,27 +4852,8 @@
       <c r="Y62" t="s">
         <v>157</v>
       </c>
-      <c r="AB62">
-        <f t="shared" si="0"/>
-        <v>3.2365496175368347</v>
-      </c>
-      <c r="AC62" t="s">
-        <v>230</v>
-      </c>
-      <c r="AD62" cm="1">
-        <f t="array" ref="AD62">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC62,"")))</f>
-        <v>174</v>
-      </c>
-      <c r="AE62" cm="1">
-        <f t="array" ref="AE62">AD62/SUM(LEN($Y$7:$Y$1005))</f>
-        <v>8.3493282149712092E-2</v>
-      </c>
-      <c r="AF62">
-        <f t="shared" si="5"/>
-        <v>8.3493282149712087</v>
-      </c>
-    </row>
-    <row r="63" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:25" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>158</v>
       </c>
@@ -5108,7 +4880,7 @@
         <v>40.615000000000002</v>
       </c>
       <c r="K63" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1977</v>
       </c>
       <c r="L63" s="9">
@@ -5147,27 +4919,8 @@
       <c r="Y63" t="s">
         <v>160</v>
       </c>
-      <c r="AB63">
-        <f t="shared" si="0"/>
-        <v>4.5634831460674157</v>
-      </c>
-      <c r="AC63" t="s">
-        <v>231</v>
-      </c>
-      <c r="AD63" cm="1">
-        <f t="array" ref="AD63">SUM(LEN($Y$2:$Y$83) - LEN(SUBSTITUTE($Y$2:$Y$83,AC63,"")))</f>
-        <v>232</v>
-      </c>
-      <c r="AE63" cm="1">
-        <f t="array" ref="AE63">AD63/SUM(LEN($Y$8:$Y$1006))</f>
-        <v>0.11383709519136408</v>
-      </c>
-      <c r="AF63">
-        <f t="shared" si="5"/>
-        <v>11.383709519136408</v>
-      </c>
-    </row>
-    <row r="64" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>161</v>
       </c>
@@ -5200,12 +4953,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>163</v>
       </c>
@@ -5239,7 +4992,7 @@
         <v>52.503999999999998</v>
       </c>
       <c r="K67" s="9">
-        <f t="shared" ref="K67" si="8">LARGE(L67:N67, 1)</f>
+        <f t="shared" ref="K67" si="6">LARGE(L67:N67, 1)</f>
         <v>1298</v>
       </c>
       <c r="L67" s="9">
@@ -5279,12 +5032,8 @@
       <c r="Y67" t="s">
         <v>164</v>
       </c>
-      <c r="AB67">
-        <f t="shared" ref="AB67:AB83" si="9">J67/D67</f>
-        <v>4.0064097672644028</v>
-      </c>
-    </row>
-    <row r="68" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>165</v>
       </c>
@@ -5338,7 +5087,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>167</v>
       </c>
@@ -5372,7 +5121,7 @@
         <v>58.816666666666663</v>
       </c>
       <c r="K69" s="9">
-        <f t="shared" ref="K69" si="10">LARGE(L69:N69, 1)</f>
+        <f t="shared" ref="K69" si="7">LARGE(L69:N69, 1)</f>
         <v>1091</v>
       </c>
       <c r="L69" s="9">
@@ -5412,12 +5161,8 @@
       <c r="Y69" t="s">
         <v>168</v>
       </c>
-      <c r="AB69">
-        <f t="shared" si="9"/>
-        <v>4.3814560985299957</v>
-      </c>
-    </row>
-    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>169</v>
       </c>
@@ -5451,7 +5196,7 @@
         <v>49.115999999999993</v>
       </c>
       <c r="K70" s="9">
-        <f t="shared" ref="K70" si="11">LARGE(L70:N70, 1)</f>
+        <f t="shared" ref="K70" si="8">LARGE(L70:N70, 1)</f>
         <v>1138</v>
       </c>
       <c r="L70" s="9">
@@ -5491,12 +5236,8 @@
       <c r="Y70" t="s">
         <v>170</v>
       </c>
-      <c r="AB70">
-        <f t="shared" si="9"/>
-        <v>4.1235832423809917</v>
-      </c>
-    </row>
-    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>171</v>
       </c>
@@ -5530,7 +5271,7 @@
         <v>37.56066666666667</v>
       </c>
       <c r="K71" s="9">
-        <f t="shared" ref="K71:K73" si="12">LARGE(L71:N71, 1)</f>
+        <f t="shared" ref="K71:K73" si="9">LARGE(L71:N71, 1)</f>
         <v>1138</v>
       </c>
       <c r="L71" s="9">
@@ -5570,12 +5311,8 @@
       <c r="Y71" t="s">
         <v>172</v>
       </c>
-      <c r="AB71">
-        <f t="shared" si="9"/>
-        <v>4.3553648732220163</v>
-      </c>
-    </row>
-    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>173</v>
       </c>
@@ -5626,7 +5363,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>175</v>
       </c>
@@ -5660,7 +5397,7 @@
         <v>67.518333333333331</v>
       </c>
       <c r="K73" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="9"/>
         <v>1495</v>
       </c>
       <c r="L73" s="9">
@@ -5700,12 +5437,8 @@
       <c r="Y73" t="s">
         <v>176</v>
       </c>
-      <c r="AB73">
-        <f t="shared" si="9"/>
-        <v>3.4598172346058584</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>177</v>
       </c>
@@ -5759,7 +5492,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>180</v>
       </c>
@@ -5813,7 +5546,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>182</v>
       </c>
@@ -5847,7 +5580,7 @@
         <v>39.847000000000001</v>
       </c>
       <c r="K76" s="9">
-        <f t="shared" ref="K76" si="13">LARGE(L76:N76, 1)</f>
+        <f t="shared" ref="K76" si="10">LARGE(L76:N76, 1)</f>
         <v>1595</v>
       </c>
       <c r="L76" s="9">
@@ -5887,17 +5620,13 @@
       <c r="Y76" t="s">
         <v>183</v>
       </c>
-      <c r="AB76">
-        <f t="shared" si="9"/>
-        <v>4.1446848346161849</v>
-      </c>
-    </row>
-    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>185</v>
       </c>
@@ -5931,7 +5660,7 @@
         <v>22.869666666666664</v>
       </c>
       <c r="K79" s="9">
-        <f t="shared" ref="K79" si="14">LARGE(L79:N79, 1)</f>
+        <f t="shared" ref="K79" si="11">LARGE(L79:N79, 1)</f>
         <v>1293</v>
       </c>
       <c r="L79" s="9">
@@ -5971,12 +5700,8 @@
       <c r="Y79" t="s">
         <v>186</v>
       </c>
-      <c r="AB79">
-        <f t="shared" si="9"/>
-        <v>3.7174360641525785</v>
-      </c>
-    </row>
-    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>187</v>
       </c>
@@ -6010,7 +5735,7 @@
         <v>21.558000000000003</v>
       </c>
       <c r="K80" s="9">
-        <f t="shared" ref="K80" si="15">LARGE(L80:N80, 1)</f>
+        <f t="shared" ref="K80" si="12">LARGE(L80:N80, 1)</f>
         <v>1279</v>
       </c>
       <c r="L80" s="9">
@@ -6050,12 +5775,8 @@
       <c r="Y80" t="s">
         <v>188</v>
       </c>
-      <c r="AB80">
-        <f t="shared" si="9"/>
-        <v>3.9738248847926276</v>
-      </c>
-    </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>189</v>
       </c>
@@ -6089,7 +5810,7 @@
         <v>24.533666666666665</v>
       </c>
       <c r="K81" s="9">
-        <f t="shared" ref="K81" si="16">LARGE(L81:N81, 1)</f>
+        <f t="shared" ref="K81" si="13">LARGE(L81:N81, 1)</f>
         <v>1256</v>
       </c>
       <c r="L81" s="9">
@@ -6129,12 +5850,8 @@
       <c r="Y81" t="s">
         <v>190</v>
       </c>
-      <c r="AB81">
-        <f t="shared" si="9"/>
-        <v>5.011985018726592</v>
-      </c>
-    </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>191</v>
       </c>
@@ -6185,7 +5902,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>193</v>
       </c>
@@ -6219,7 +5936,7 @@
         <v>20.844333333333331</v>
       </c>
       <c r="K83" s="9">
-        <f t="shared" ref="K83" si="17">LARGE(L83:N83, 1)</f>
+        <f t="shared" ref="K83" si="14">LARGE(L83:N83, 1)</f>
         <v>1208</v>
       </c>
       <c r="L83" s="9">
@@ -6259,26 +5976,9 @@
       <c r="Y83" t="s">
         <v>194</v>
       </c>
-      <c r="AB83">
-        <f t="shared" si="9"/>
-        <v>3.8422734254992319</v>
-      </c>
-    </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D85">
-        <f>PEARSON(D2:D83, I2:I83)</f>
-        <v>0.93345351774539209</v>
-      </c>
-      <c r="AB85">
-        <f>AVERAGE(AB2:AB83)</f>
-        <v>4.1996213888627274</v>
-      </c>
-    </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="O87" s="9">
-        <f>AVERAGE(O2:O83,'Rules 2'!O2:O11)</f>
-        <v>1166.2138364779876</v>
-      </c>
+    </row>
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D85"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C17 C20:C1048576">
@@ -6329,16 +6029,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -6577,31 +6277,31 @@
         <v>195</v>
       </c>
       <c r="M2" s="14">
-        <f>B2/$I2</f>
+        <f t="shared" ref="M2:S8" si="0">B2/$I2</f>
         <v>0.1736111111111111</v>
       </c>
       <c r="N2" s="14">
-        <f>C2/$I2</f>
+        <f t="shared" si="0"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="O2" s="14">
-        <f>D2/$I2</f>
+        <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
       <c r="P2" s="14">
-        <f>E2/$I2</f>
+        <f t="shared" si="0"/>
         <v>0.27777777777777779</v>
       </c>
       <c r="Q2" s="14">
-        <f>F2/$I2</f>
+        <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
       </c>
       <c r="R2" s="14">
-        <f>G2/$I2</f>
+        <f t="shared" si="0"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="S2" s="14">
-        <f>H2/$I2</f>
+        <f t="shared" si="0"/>
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
@@ -6637,31 +6337,31 @@
         <v>196</v>
       </c>
       <c r="M3" s="14">
-        <f>B3/$I3</f>
+        <f t="shared" si="0"/>
         <v>0.36585365853658536</v>
       </c>
       <c r="N3" s="14">
-        <f>C3/$I3</f>
+        <f t="shared" si="0"/>
         <v>0.32520325203252032</v>
       </c>
       <c r="O3" s="14">
-        <f>D3/$I3</f>
+        <f t="shared" si="0"/>
         <v>4.065040650406504E-2</v>
       </c>
       <c r="P3" s="14">
-        <f>E3/$I3</f>
+        <f t="shared" si="0"/>
         <v>0.24390243902439024</v>
       </c>
       <c r="Q3" s="14">
-        <f>F3/$I3</f>
+        <f t="shared" si="0"/>
         <v>2.4390243902439025E-2</v>
       </c>
       <c r="R3" s="14">
-        <f>G3/$I3</f>
+        <f t="shared" si="0"/>
         <v>1.6260162601626018E-2</v>
       </c>
       <c r="S3" s="14">
-        <f>H3/$I3</f>
+        <f t="shared" si="0"/>
         <v>1.6260162601626018E-2</v>
       </c>
     </row>
@@ -6697,31 +6397,31 @@
         <v>197</v>
       </c>
       <c r="M4" s="14">
-        <f>B4/$I4</f>
+        <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="N4" s="14">
-        <f>C4/$I4</f>
+        <f t="shared" si="0"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="O4" s="14">
-        <f>D4/$I4</f>
+        <f t="shared" si="0"/>
         <v>0.30303030303030304</v>
       </c>
       <c r="P4" s="14">
-        <f>E4/$I4</f>
+        <f t="shared" si="0"/>
         <v>6.0606060606060608E-2</v>
       </c>
       <c r="Q4" s="14">
-        <f>F4/$I4</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R4" s="14">
-        <f>G4/$I4</f>
+        <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="S4" s="14">
-        <f>H4/$I4</f>
+        <f t="shared" si="0"/>
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
@@ -6757,31 +6457,31 @@
         <v>198</v>
       </c>
       <c r="M5" s="14">
-        <f>B5/$I5</f>
+        <f t="shared" si="0"/>
         <v>0.46391752577319589</v>
       </c>
       <c r="N5" s="14">
-        <f>C5/$I5</f>
+        <f t="shared" si="0"/>
         <v>0.25773195876288657</v>
       </c>
       <c r="O5" s="14">
-        <f>D5/$I5</f>
+        <f t="shared" si="0"/>
         <v>3.0927835051546393E-2</v>
       </c>
       <c r="P5" s="14">
-        <f>E5/$I5</f>
+        <f t="shared" si="0"/>
         <v>0.36082474226804123</v>
       </c>
       <c r="Q5" s="14">
-        <f>F5/$I5</f>
+        <f t="shared" si="0"/>
         <v>5.1546391752577317E-2</v>
       </c>
       <c r="R5" s="14">
-        <f>G5/$I5</f>
+        <f t="shared" si="0"/>
         <v>1.0309278350515464E-2</v>
       </c>
       <c r="S5" s="14">
-        <f>H5/$I5</f>
+        <f t="shared" si="0"/>
         <v>1.0309278350515464E-2</v>
       </c>
     </row>
@@ -6817,31 +6517,31 @@
         <v>199</v>
       </c>
       <c r="M6" s="14">
-        <f>B6/$I6</f>
+        <f t="shared" si="0"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="N6" s="14">
-        <f>C6/$I6</f>
+        <f t="shared" si="0"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="O6" s="14">
-        <f>D6/$I6</f>
+        <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="P6" s="14">
-        <f>E6/$I6</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="Q6" s="14">
-        <f>F6/$I6</f>
+        <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R6" s="14">
-        <f>G6/$I6</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="S6" s="14">
-        <f>H6/$I6</f>
+        <f t="shared" si="0"/>
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
@@ -6877,31 +6577,31 @@
         <v>200</v>
       </c>
       <c r="M7" s="14">
-        <f>B7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="N7" s="14">
-        <f>C7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O7" s="14">
-        <f>D7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="P7" s="14">
-        <f>E7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="Q7" s="14">
-        <f>F7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="R7" s="14">
-        <f>G7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="S7" s="14">
-        <f>H7/$I7</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -6937,31 +6637,31 @@
         <v>201</v>
       </c>
       <c r="M8" s="14">
-        <f>B8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="N8" s="14">
-        <f>C8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="O8" s="14">
-        <f>D8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P8" s="14">
-        <f>E8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="Q8" s="14">
-        <f>F8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R8" s="14">
-        <f>G8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S8" s="14">
-        <f>H8/$I8</f>
+        <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -6973,11 +6673,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E3BC3-0E55-4707-8A33-8D76B8D2F300}">
-  <dimension ref="A1:AA83"/>
+  <dimension ref="A1:Y83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="AA11" sqref="AA2:AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7007,7 +6707,7 @@
     <col min="25" max="25" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7084,7 +6784,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>202</v>
       </c>
@@ -7158,12 +6858,8 @@
       <c r="Y2" t="s">
         <v>205</v>
       </c>
-      <c r="AA2">
-        <f>J2/D2</f>
-        <v>4.3647027099905618</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>203</v>
       </c>
@@ -7240,12 +6936,8 @@
       <c r="Y3" t="s">
         <v>204</v>
       </c>
-      <c r="AA3">
-        <f t="shared" ref="AA3:AA11" si="0">J3/D3</f>
-        <v>4.3904811837352895</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -7319,12 +7011,8 @@
       <c r="Y4" t="s">
         <v>208</v>
       </c>
-      <c r="AA4">
-        <f t="shared" si="0"/>
-        <v>4.0950592443550189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>209</v>
       </c>
@@ -7375,7 +7063,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -7392,7 +7080,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="7">
-        <f t="shared" ref="F6:F11" si="1">SUM(G6:I6)</f>
+        <f t="shared" ref="F6:F11" si="0">SUM(G6:I6)</f>
         <v>221.18100000000001</v>
       </c>
       <c r="G6" s="7">
@@ -7405,11 +7093,11 @@
         <v>59.220999999999997</v>
       </c>
       <c r="J6" s="7">
-        <f t="shared" ref="J6:J11" si="2">AVERAGE(G6:I6)</f>
+        <f t="shared" ref="J6:J11" si="1">AVERAGE(G6:I6)</f>
         <v>73.727000000000004</v>
       </c>
       <c r="K6" s="9">
-        <f t="shared" ref="K6:K11" si="3">LARGE(L6:N6, 1)</f>
+        <f t="shared" ref="K6:K11" si="2">LARGE(L6:N6, 1)</f>
         <v>1432</v>
       </c>
       <c r="L6" s="9">
@@ -7422,7 +7110,7 @@
         <v>1432</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" ref="O6:O11" si="4">AVERAGE(L6:N6)</f>
+        <f t="shared" ref="O6:O11" si="3">AVERAGE(L6:N6)</f>
         <v>1219</v>
       </c>
       <c r="P6" s="10">
@@ -7449,12 +7137,8 @@
       <c r="Y6" t="s">
         <v>212</v>
       </c>
-      <c r="AA6">
-        <f t="shared" si="0"/>
-        <v>3.5774176330729293</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>213</v>
       </c>
@@ -7471,7 +7155,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>124.577</v>
       </c>
       <c r="G7" s="7">
@@ -7484,11 +7168,11 @@
         <v>40.520000000000003</v>
       </c>
       <c r="J7" s="7">
+        <f t="shared" si="1"/>
+        <v>41.525666666666666</v>
+      </c>
+      <c r="K7" s="9">
         <f t="shared" si="2"/>
-        <v>41.525666666666666</v>
-      </c>
-      <c r="K7" s="9">
-        <f t="shared" si="3"/>
         <v>1422</v>
       </c>
       <c r="L7" s="9">
@@ -7501,7 +7185,7 @@
         <v>1129</v>
       </c>
       <c r="O7" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1185.3333333333333</v>
       </c>
       <c r="P7" s="10">
@@ -7528,12 +7212,8 @@
       <c r="Y7" t="s">
         <v>214</v>
       </c>
-      <c r="AA7">
-        <f t="shared" si="0"/>
-        <v>4.2269611834961998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -7563,11 +7243,11 @@
         <v>43.02</v>
       </c>
       <c r="J8" s="7">
+        <f t="shared" si="1"/>
+        <v>40.969666666666662</v>
+      </c>
+      <c r="K8" s="9">
         <f t="shared" si="2"/>
-        <v>40.969666666666662</v>
-      </c>
-      <c r="K8" s="9">
-        <f t="shared" si="3"/>
         <v>969</v>
       </c>
       <c r="L8" s="9">
@@ -7580,7 +7260,7 @@
         <v>969</v>
       </c>
       <c r="O8" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>889.66666666666663</v>
       </c>
       <c r="P8" s="10">
@@ -7610,12 +7290,8 @@
       <c r="Y8" t="s">
         <v>216</v>
       </c>
-      <c r="AA8">
-        <f t="shared" si="0"/>
-        <v>4.6614707778662714</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>219</v>
       </c>
@@ -7632,7 +7308,7 @@
         <v>24</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>148.999</v>
       </c>
       <c r="G9" s="7">
@@ -7645,11 +7321,11 @@
         <v>44.28</v>
       </c>
       <c r="J9" s="7">
+        <f t="shared" si="1"/>
+        <v>49.666333333333334</v>
+      </c>
+      <c r="K9" s="9">
         <f t="shared" si="2"/>
-        <v>49.666333333333334</v>
-      </c>
-      <c r="K9" s="9">
-        <f t="shared" si="3"/>
         <v>1313</v>
       </c>
       <c r="L9" s="9">
@@ -7662,7 +7338,7 @@
         <v>1313</v>
       </c>
       <c r="O9" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1213.3333333333333</v>
       </c>
       <c r="P9" s="10">
@@ -7692,12 +7368,8 @@
       <c r="Y9" t="s">
         <v>220</v>
       </c>
-      <c r="AA9">
-        <f t="shared" si="0"/>
-        <v>3.7685965045400511</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>221</v>
       </c>
@@ -7714,7 +7386,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>185.63499999999999</v>
       </c>
       <c r="G10" s="7">
@@ -7727,11 +7399,11 @@
         <v>55.158999999999999</v>
       </c>
       <c r="J10" s="7">
+        <f t="shared" si="1"/>
+        <v>61.87833333333333</v>
+      </c>
+      <c r="K10" s="9">
         <f t="shared" si="2"/>
-        <v>61.87833333333333</v>
-      </c>
-      <c r="K10" s="9">
-        <f t="shared" si="3"/>
         <v>1229</v>
       </c>
       <c r="L10" s="9">
@@ -7744,7 +7416,7 @@
         <v>1195</v>
       </c>
       <c r="O10" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1206.3333333333333</v>
       </c>
       <c r="P10" s="10">
@@ -7771,12 +7443,8 @@
       <c r="Y10" t="s">
         <v>222</v>
       </c>
-      <c r="AA10">
-        <f t="shared" si="0"/>
-        <v>3.9327782721071141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>223</v>
       </c>
@@ -7793,7 +7461,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>266.74199999999996</v>
       </c>
       <c r="G11" s="7">
@@ -7806,11 +7474,11 @@
         <v>86.218999999999994</v>
       </c>
       <c r="J11" s="7">
+        <f t="shared" si="1"/>
+        <v>88.913999999999987</v>
+      </c>
+      <c r="K11" s="9">
         <f t="shared" si="2"/>
-        <v>88.913999999999987</v>
-      </c>
-      <c r="K11" s="9">
-        <f t="shared" si="3"/>
         <v>1152</v>
       </c>
       <c r="L11" s="9">
@@ -7823,7 +7491,7 @@
         <v>1062</v>
       </c>
       <c r="O11" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1071.3333333333333</v>
       </c>
       <c r="P11" s="10">
@@ -7850,12 +7518,8 @@
       <c r="Y11" t="s">
         <v>224</v>
       </c>
-      <c r="AA11">
-        <f t="shared" si="0"/>
-        <v>4.3491488945411856</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="D13"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -8052,16 +7716,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -8189,15 +7853,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010091DF57B0FF84684F9DCA854C9FFB8912" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d39cd055a4764590ebe89418264d1cee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3ca4e8a-6c47-4ee3-b5a2-c9cd7b599a4c" xmlns:ns3="fd2277a0-dc9c-4a4f-b323-d8f3f426fdeb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e621e2cb76b7ddaa2f9a50fca7ca654" ns2:_="" ns3:_="">
     <xsd:import namespace="c3ca4e8a-6c47-4ee3-b5a2-c9cd7b599a4c"/>
@@ -8420,15 +8075,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{972B5B9A-003C-403E-8E04-35446E48BD5F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82F372BC-C340-4FFA-BD5C-A3498EBF99B6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8445,4 +8101,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{972B5B9A-003C-403E-8E04-35446E48BD5F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>